<commit_message>
Changed ID in Spreadsheet
</commit_message>
<xml_diff>
--- a/resources/ChromeTest.xlsx
+++ b/resources/ChromeTest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\Workspace\AndroidTestProject\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Workspace\AppiumProject\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>DeviceId</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Kingdom Hearts HD 1.5 + 2.5 ReMIX - PlayStation 4</t>
-  </si>
-  <si>
-    <t>10.255.191.231:5556</t>
   </si>
   <si>
     <t>TargetURL</t>
@@ -458,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,25 +472,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>2</v>
@@ -504,31 +501,31 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
         <v>4</v>
@@ -538,12 +535,6 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
       <c r="K3" t="s">
         <v>4</v>
       </c>

</xml_diff>